<commit_message>
PCA, MCA Analysis Factorielle
</commit_message>
<xml_diff>
--- a/EXPLORATION/Autos_Mixtes.xlsx
+++ b/EXPLORATION/Autos_Mixtes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmezghani/Dropbox/EnseignementBdeB/Cours420-A55-BB/Cours 7 - AFDM/Programme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valm044\IACollege\EXPLORATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7655FC3A-1C62-E44E-B9F9-1337392B1D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0532D099-B654-4B5B-AE56-39233BC19257}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="3260" windowWidth="27240" windowHeight="16440" xr2:uid="{92510EDD-9B12-8E45-8531-9FE1E929F6CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{92510EDD-9B12-8E45-8531-9FE1E929F6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="types" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -23,10 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Modele</t>
   </si>
@@ -112,13 +110,46 @@
   </si>
   <si>
     <t xml:space="preserve">SANTA_FE    </t>
+  </si>
+  <si>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>type de variable</t>
+  </si>
+  <si>
+    <t>Qualitative</t>
+  </si>
+  <si>
+    <t>CYL</t>
+  </si>
+  <si>
+    <t>Quantitative</t>
+  </si>
+  <si>
+    <t>PUISS</t>
+  </si>
+  <si>
+    <t>LONG</t>
+  </si>
+  <si>
+    <t>LARG</t>
+  </si>
+  <si>
+    <t>POIDS</t>
+  </si>
+  <si>
+    <t>V.MAX</t>
+  </si>
+  <si>
+    <t>Origine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,8 +157,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Bitstream Vera Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +197,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -176,20 +233,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{CD4ABEC7-451A-44CF-9C70-4EA0F06650DB}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -210,7 +283,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -508,13 +581,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0415AA-9045-4E40-B601-BE3B2BB9228E}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -543,7 +616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -572,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -601,7 +674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -630,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -659,7 +732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -688,7 +761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -717,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -746,7 +819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -775,7 +848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -804,7 +877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -835,5 +908,122 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CC2225-8221-44AF-88D4-1CAA823DC8C1}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>